<commit_message>
Basic search with any keywords
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="168">
   <si>
     <t>plot_total_sale_inv_bydf</t>
   </si>
@@ -504,13 +504,7 @@
     <t>SALES YEARLY TREND</t>
   </si>
   <si>
-    <t>Search by</t>
-  </si>
-  <si>
     <t>Store Name</t>
-  </si>
-  <si>
-    <t>Select year</t>
   </si>
   <si>
     <t>Result</t>
@@ -981,27 +975,78 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1010,57 +1055,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3404,730 +3398,710 @@
       <c r="A1" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="53" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53" t="s">
+      <c r="H1" s="76"/>
+      <c r="I1" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53" t="s">
+      <c r="J1" s="76"/>
+      <c r="K1" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="53"/>
+      <c r="L1" s="76"/>
       <c r="N1" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="O1" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53" t="s">
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53" t="s">
+      <c r="U1" s="76"/>
+      <c r="V1" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53" t="s">
+      <c r="W1" s="76"/>
+      <c r="X1" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="Y1" s="53"/>
+      <c r="Y1" s="76"/>
     </row>
     <row r="2" spans="1:25" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68"/>
-      <c r="B2" s="70" t="s">
+      <c r="A2" s="70"/>
+      <c r="B2" s="72" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="69"/>
-      <c r="N2" s="54" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="71"/>
+      <c r="N2" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="54" t="s">
+      <c r="O2" s="65"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="54" t="s">
+      <c r="R2" s="65"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="U2" s="55"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="54" t="s">
+      <c r="U2" s="65"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="56"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="66"/>
     </row>
     <row r="3" spans="1:25" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="67" t="s">
+      <c r="A3" s="70"/>
+      <c r="B3" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="69"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="59"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="71"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="68"/>
+      <c r="Y3" s="69"/>
     </row>
     <row r="4" spans="1:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="68"/>
-      <c r="B4" s="71" t="s">
+      <c r="A4" s="70"/>
+      <c r="B4" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="69"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="71"/>
       <c r="N4" s="38"/>
-      <c r="O4" s="72" t="s">
+      <c r="O4" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="75"/>
       <c r="Y4" s="38"/>
     </row>
     <row r="5" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68"/>
-      <c r="B5" s="67" t="s">
+      <c r="A5" s="70"/>
+      <c r="B5" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="69"/>
-      <c r="N5" s="63" t="s">
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="71"/>
+      <c r="N5" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="67" t="s">
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="67"/>
-      <c r="W5" s="64" t="s">
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="75"/>
+      <c r="X5" s="57"/>
+      <c r="Y5" s="58"/>
     </row>
     <row r="6" spans="1:25" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="68"/>
-      <c r="B6" s="71" t="s">
+      <c r="A6" s="70"/>
+      <c r="B6" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="69"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="76"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="71"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="60"/>
+      <c r="X6" s="60"/>
+      <c r="Y6" s="61"/>
     </row>
     <row r="7" spans="1:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="68"/>
-      <c r="B7" s="67" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="69"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="71"/>
       <c r="N7" s="38"/>
-      <c r="O7" s="71" t="s">
+      <c r="O7" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="P7" s="71"/>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
-      <c r="S7" s="71"/>
-      <c r="T7" s="71"/>
-      <c r="U7" s="71"/>
-      <c r="V7" s="71"/>
-      <c r="W7" s="71"/>
-      <c r="X7" s="71"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
       <c r="Y7" s="38"/>
     </row>
     <row r="8" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N8" s="67" t="s">
+      <c r="N8" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="67"/>
-      <c r="T8" s="67" t="s">
+      <c r="O8" s="62"/>
+      <c r="P8" s="62"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="U8" s="67"/>
-      <c r="V8" s="67"/>
-      <c r="W8" s="67"/>
-      <c r="X8" s="67"/>
-      <c r="Y8" s="67"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="62"/>
+      <c r="W8" s="62"/>
+      <c r="X8" s="62"/>
+      <c r="Y8" s="62"/>
     </row>
     <row r="9" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="39"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
-      <c r="R9" s="67"/>
-      <c r="S9" s="67"/>
-      <c r="T9" s="67"/>
-      <c r="U9" s="67"/>
-      <c r="V9" s="67"/>
-      <c r="W9" s="67"/>
-      <c r="X9" s="67"/>
-      <c r="Y9" s="67"/>
+      <c r="N9" s="62"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="62"/>
     </row>
     <row r="10" spans="1:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N10" s="38"/>
-      <c r="O10" s="71" t="s">
+      <c r="O10" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="P10" s="71"/>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="71"/>
-      <c r="S10" s="71"/>
-      <c r="T10" s="71"/>
-      <c r="U10" s="71"/>
-      <c r="V10" s="71"/>
-      <c r="W10" s="71"/>
-      <c r="X10" s="71"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
       <c r="Y10" s="38"/>
     </row>
     <row r="11" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N11" s="63" t="s">
+      <c r="N11" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="O11" s="64"/>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="64"/>
-      <c r="S11" s="75"/>
-      <c r="T11" s="63" t="s">
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="U11" s="64"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="64"/>
-      <c r="X11" s="64"/>
-      <c r="Y11" s="75"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
+      <c r="Y11" s="58"/>
     </row>
     <row r="12" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N12" s="65"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="76"/>
-      <c r="T12" s="65"/>
-      <c r="U12" s="66"/>
-      <c r="V12" s="66"/>
-      <c r="W12" s="66"/>
-      <c r="X12" s="66"/>
-      <c r="Y12" s="76"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="60"/>
+      <c r="V12" s="60"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="61"/>
     </row>
     <row r="13" spans="1:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N13" s="38"/>
-      <c r="O13" s="77" t="s">
+      <c r="O13" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="78"/>
-      <c r="R13" s="78"/>
-      <c r="S13" s="78"/>
-      <c r="T13" s="78"/>
-      <c r="U13" s="78"/>
-      <c r="V13" s="78"/>
-      <c r="W13" s="78"/>
-      <c r="X13" s="79"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="54"/>
+      <c r="U13" s="54"/>
+      <c r="V13" s="54"/>
+      <c r="W13" s="54"/>
+      <c r="X13" s="55"/>
       <c r="Y13" s="38"/>
     </row>
     <row r="14" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N14" s="63" t="s">
+      <c r="N14" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="64"/>
-      <c r="S14" s="75"/>
-      <c r="T14" s="63" t="s">
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="U14" s="64"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="64"/>
-      <c r="X14" s="64"/>
-      <c r="Y14" s="75"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
+      <c r="Y14" s="58"/>
     </row>
     <row r="15" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N15" s="65"/>
-      <c r="O15" s="66"/>
-      <c r="P15" s="66"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="66"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="65"/>
-      <c r="U15" s="66"/>
-      <c r="V15" s="66"/>
-      <c r="W15" s="66"/>
-      <c r="X15" s="66"/>
-      <c r="Y15" s="76"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="59"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="60"/>
+      <c r="X15" s="60"/>
+      <c r="Y15" s="61"/>
     </row>
     <row r="16" spans="1:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N16" s="38"/>
-      <c r="O16" s="77" t="s">
+      <c r="O16" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="78"/>
-      <c r="S16" s="78"/>
-      <c r="T16" s="78"/>
-      <c r="U16" s="78"/>
-      <c r="V16" s="78"/>
-      <c r="W16" s="78"/>
-      <c r="X16" s="79"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="54"/>
+      <c r="T16" s="54"/>
+      <c r="U16" s="54"/>
+      <c r="V16" s="54"/>
+      <c r="W16" s="54"/>
+      <c r="X16" s="55"/>
       <c r="Y16" s="38"/>
     </row>
     <row r="17" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N17" s="63" t="s">
+      <c r="N17" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="O17" s="64"/>
-      <c r="P17" s="64"/>
-      <c r="Q17" s="64"/>
-      <c r="R17" s="64"/>
-      <c r="S17" s="75"/>
-      <c r="T17" s="63" t="s">
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="57"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="U17" s="64"/>
-      <c r="V17" s="64"/>
-      <c r="W17" s="64"/>
-      <c r="X17" s="64"/>
-      <c r="Y17" s="75"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
+      <c r="Y17" s="58"/>
     </row>
     <row r="18" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N18" s="65"/>
-      <c r="O18" s="66"/>
-      <c r="P18" s="66"/>
-      <c r="Q18" s="66"/>
-      <c r="R18" s="66"/>
-      <c r="S18" s="76"/>
-      <c r="T18" s="65"/>
-      <c r="U18" s="66"/>
-      <c r="V18" s="66"/>
-      <c r="W18" s="66"/>
-      <c r="X18" s="66"/>
-      <c r="Y18" s="76"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="61"/>
     </row>
     <row r="19" spans="14:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N19" s="38"/>
-      <c r="O19" s="77" t="s">
+      <c r="O19" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="P19" s="78"/>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="78"/>
-      <c r="S19" s="78"/>
-      <c r="T19" s="78"/>
-      <c r="U19" s="78"/>
-      <c r="V19" s="78"/>
-      <c r="W19" s="78"/>
-      <c r="X19" s="79"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
+      <c r="T19" s="54"/>
+      <c r="U19" s="54"/>
+      <c r="V19" s="54"/>
+      <c r="W19" s="54"/>
+      <c r="X19" s="55"/>
       <c r="Y19" s="38"/>
     </row>
     <row r="20" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N20" s="63" t="s">
+      <c r="N20" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="O20" s="64"/>
-      <c r="P20" s="64"/>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="75"/>
-      <c r="T20" s="63" t="s">
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="U20" s="64"/>
-      <c r="V20" s="64"/>
-      <c r="W20" s="64"/>
-      <c r="X20" s="64"/>
-      <c r="Y20" s="75"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="58"/>
     </row>
     <row r="21" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N21" s="65"/>
-      <c r="O21" s="66"/>
-      <c r="P21" s="66"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="66"/>
-      <c r="S21" s="76"/>
-      <c r="T21" s="65"/>
-      <c r="U21" s="66"/>
-      <c r="V21" s="66"/>
-      <c r="W21" s="66"/>
-      <c r="X21" s="66"/>
-      <c r="Y21" s="76"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="61"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="60"/>
+      <c r="X21" s="60"/>
+      <c r="Y21" s="61"/>
     </row>
     <row r="22" spans="14:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N22" s="38"/>
-      <c r="O22" s="77" t="s">
+      <c r="O22" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="P22" s="78"/>
-      <c r="Q22" s="78"/>
-      <c r="R22" s="78"/>
-      <c r="S22" s="78"/>
-      <c r="T22" s="78"/>
-      <c r="U22" s="78"/>
-      <c r="V22" s="78"/>
-      <c r="W22" s="78"/>
-      <c r="X22" s="79"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
+      <c r="T22" s="54"/>
+      <c r="U22" s="54"/>
+      <c r="V22" s="54"/>
+      <c r="W22" s="54"/>
+      <c r="X22" s="55"/>
       <c r="Y22" s="38"/>
     </row>
     <row r="23" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N23" s="63" t="s">
+      <c r="N23" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="O23" s="64"/>
-      <c r="P23" s="64"/>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="64"/>
-      <c r="S23" s="75"/>
-      <c r="T23" s="63" t="s">
+      <c r="O23" s="57"/>
+      <c r="P23" s="57"/>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="U23" s="64"/>
-      <c r="V23" s="64"/>
-      <c r="W23" s="64"/>
-      <c r="X23" s="64"/>
-      <c r="Y23" s="75"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="58"/>
     </row>
     <row r="24" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N24" s="65"/>
-      <c r="O24" s="66"/>
-      <c r="P24" s="66"/>
-      <c r="Q24" s="66"/>
-      <c r="R24" s="66"/>
-      <c r="S24" s="76"/>
-      <c r="T24" s="65"/>
-      <c r="U24" s="66"/>
-      <c r="V24" s="66"/>
-      <c r="W24" s="66"/>
-      <c r="X24" s="66"/>
-      <c r="Y24" s="76"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="61"/>
+      <c r="T24" s="59"/>
+      <c r="U24" s="60"/>
+      <c r="V24" s="60"/>
+      <c r="W24" s="60"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="61"/>
     </row>
     <row r="25" spans="14:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N25" s="38"/>
-      <c r="O25" s="77" t="s">
+      <c r="O25" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="78"/>
-      <c r="S25" s="78"/>
-      <c r="T25" s="78"/>
-      <c r="U25" s="78"/>
-      <c r="V25" s="78"/>
-      <c r="W25" s="78"/>
-      <c r="X25" s="79"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="54"/>
+      <c r="T25" s="54"/>
+      <c r="U25" s="54"/>
+      <c r="V25" s="54"/>
+      <c r="W25" s="54"/>
+      <c r="X25" s="55"/>
       <c r="Y25" s="38"/>
     </row>
     <row r="26" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N26" s="63" t="s">
+      <c r="N26" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="O26" s="64"/>
-      <c r="P26" s="64"/>
-      <c r="Q26" s="64"/>
-      <c r="R26" s="64"/>
-      <c r="S26" s="75"/>
-      <c r="T26" s="63" t="s">
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="57"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="U26" s="64"/>
-      <c r="V26" s="64"/>
-      <c r="W26" s="64"/>
-      <c r="X26" s="64"/>
-      <c r="Y26" s="75"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="58"/>
     </row>
     <row r="27" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N27" s="65"/>
-      <c r="O27" s="66"/>
-      <c r="P27" s="66"/>
-      <c r="Q27" s="66"/>
-      <c r="R27" s="66"/>
-      <c r="S27" s="76"/>
-      <c r="T27" s="65"/>
-      <c r="U27" s="66"/>
-      <c r="V27" s="66"/>
-      <c r="W27" s="66"/>
-      <c r="X27" s="66"/>
-      <c r="Y27" s="76"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="60"/>
+      <c r="V27" s="60"/>
+      <c r="W27" s="60"/>
+      <c r="X27" s="60"/>
+      <c r="Y27" s="61"/>
     </row>
     <row r="28" spans="14:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N28" s="38"/>
-      <c r="O28" s="77" t="s">
+      <c r="O28" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="P28" s="78"/>
-      <c r="Q28" s="78"/>
-      <c r="R28" s="78"/>
-      <c r="S28" s="78"/>
-      <c r="T28" s="78"/>
-      <c r="U28" s="78"/>
-      <c r="V28" s="78"/>
-      <c r="W28" s="78"/>
-      <c r="X28" s="79"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
+      <c r="T28" s="54"/>
+      <c r="U28" s="54"/>
+      <c r="V28" s="54"/>
+      <c r="W28" s="54"/>
+      <c r="X28" s="55"/>
       <c r="Y28" s="38"/>
     </row>
     <row r="29" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N29" s="63" t="s">
+      <c r="N29" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="O29" s="64"/>
-      <c r="P29" s="64"/>
-      <c r="Q29" s="64"/>
-      <c r="R29" s="64"/>
-      <c r="S29" s="75"/>
-      <c r="T29" s="63" t="s">
+      <c r="O29" s="57"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="57"/>
+      <c r="R29" s="57"/>
+      <c r="S29" s="58"/>
+      <c r="T29" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="U29" s="64"/>
-      <c r="V29" s="64"/>
-      <c r="W29" s="64"/>
-      <c r="X29" s="64"/>
-      <c r="Y29" s="75"/>
+      <c r="U29" s="57"/>
+      <c r="V29" s="57"/>
+      <c r="W29" s="57"/>
+      <c r="X29" s="57"/>
+      <c r="Y29" s="58"/>
     </row>
     <row r="30" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N30" s="65"/>
-      <c r="O30" s="66"/>
-      <c r="P30" s="66"/>
-      <c r="Q30" s="66"/>
-      <c r="R30" s="66"/>
-      <c r="S30" s="76"/>
-      <c r="T30" s="65"/>
-      <c r="U30" s="66"/>
-      <c r="V30" s="66"/>
-      <c r="W30" s="66"/>
-      <c r="X30" s="66"/>
-      <c r="Y30" s="76"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="61"/>
+      <c r="T30" s="59"/>
+      <c r="U30" s="60"/>
+      <c r="V30" s="60"/>
+      <c r="W30" s="60"/>
+      <c r="X30" s="60"/>
+      <c r="Y30" s="61"/>
     </row>
     <row r="31" spans="14:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N31" s="38"/>
-      <c r="O31" s="77" t="s">
+      <c r="O31" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="P31" s="78"/>
-      <c r="Q31" s="78"/>
-      <c r="R31" s="78"/>
-      <c r="S31" s="78"/>
-      <c r="T31" s="78"/>
-      <c r="U31" s="78"/>
-      <c r="V31" s="78"/>
-      <c r="W31" s="78"/>
-      <c r="X31" s="79"/>
+      <c r="P31" s="54"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="54"/>
+      <c r="T31" s="54"/>
+      <c r="U31" s="54"/>
+      <c r="V31" s="54"/>
+      <c r="W31" s="54"/>
+      <c r="X31" s="55"/>
       <c r="Y31" s="38"/>
     </row>
     <row r="32" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N32" s="63" t="s">
+      <c r="N32" s="56" t="s">
         <v>155</v>
       </c>
-      <c r="O32" s="64"/>
-      <c r="P32" s="64"/>
-      <c r="Q32" s="64"/>
-      <c r="R32" s="64"/>
-      <c r="S32" s="75"/>
-      <c r="T32" s="63" t="s">
+      <c r="O32" s="57"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="57"/>
+      <c r="S32" s="58"/>
+      <c r="T32" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="U32" s="64"/>
-      <c r="V32" s="64"/>
-      <c r="W32" s="64"/>
-      <c r="X32" s="64"/>
-      <c r="Y32" s="75"/>
+      <c r="U32" s="57"/>
+      <c r="V32" s="57"/>
+      <c r="W32" s="57"/>
+      <c r="X32" s="57"/>
+      <c r="Y32" s="58"/>
     </row>
     <row r="33" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N33" s="65"/>
-      <c r="O33" s="66"/>
-      <c r="P33" s="66"/>
-      <c r="Q33" s="66"/>
-      <c r="R33" s="66"/>
-      <c r="S33" s="76"/>
-      <c r="T33" s="65"/>
-      <c r="U33" s="66"/>
-      <c r="V33" s="66"/>
-      <c r="W33" s="66"/>
-      <c r="X33" s="66"/>
-      <c r="Y33" s="76"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="61"/>
+      <c r="T33" s="59"/>
+      <c r="U33" s="60"/>
+      <c r="V33" s="60"/>
+      <c r="W33" s="60"/>
+      <c r="X33" s="60"/>
+      <c r="Y33" s="61"/>
     </row>
     <row r="34" spans="14:25" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N34" s="38"/>
-      <c r="O34" s="77" t="s">
+      <c r="O34" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="P34" s="78"/>
-      <c r="Q34" s="78"/>
-      <c r="R34" s="78"/>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="78"/>
-      <c r="V34" s="78"/>
-      <c r="W34" s="78"/>
-      <c r="X34" s="79"/>
+      <c r="P34" s="54"/>
+      <c r="Q34" s="54"/>
+      <c r="R34" s="54"/>
+      <c r="S34" s="54"/>
+      <c r="T34" s="54"/>
+      <c r="U34" s="54"/>
+      <c r="V34" s="54"/>
+      <c r="W34" s="54"/>
+      <c r="X34" s="55"/>
       <c r="Y34" s="38"/>
     </row>
     <row r="35" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N35" s="63" t="s">
+      <c r="N35" s="56" t="s">
         <v>155</v>
       </c>
-      <c r="O35" s="64"/>
-      <c r="P35" s="64"/>
-      <c r="Q35" s="64"/>
-      <c r="R35" s="64"/>
-      <c r="S35" s="75"/>
-      <c r="T35" s="63" t="s">
+      <c r="O35" s="57"/>
+      <c r="P35" s="57"/>
+      <c r="Q35" s="57"/>
+      <c r="R35" s="57"/>
+      <c r="S35" s="58"/>
+      <c r="T35" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="U35" s="64"/>
-      <c r="V35" s="64"/>
-      <c r="W35" s="64"/>
-      <c r="X35" s="64"/>
-      <c r="Y35" s="75"/>
+      <c r="U35" s="57"/>
+      <c r="V35" s="57"/>
+      <c r="W35" s="57"/>
+      <c r="X35" s="57"/>
+      <c r="Y35" s="58"/>
     </row>
     <row r="36" spans="14:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N36" s="65"/>
-      <c r="O36" s="66"/>
-      <c r="P36" s="66"/>
-      <c r="Q36" s="66"/>
-      <c r="R36" s="66"/>
-      <c r="S36" s="76"/>
-      <c r="T36" s="65"/>
-      <c r="U36" s="66"/>
-      <c r="V36" s="66"/>
-      <c r="W36" s="66"/>
-      <c r="X36" s="66"/>
-      <c r="Y36" s="76"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="61"/>
+      <c r="T36" s="59"/>
+      <c r="U36" s="60"/>
+      <c r="V36" s="60"/>
+      <c r="W36" s="60"/>
+      <c r="X36" s="60"/>
+      <c r="Y36" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="O34:X34"/>
-    <mergeCell ref="N35:S36"/>
-    <mergeCell ref="T35:Y36"/>
-    <mergeCell ref="N29:S30"/>
-    <mergeCell ref="T29:Y30"/>
-    <mergeCell ref="O31:X31"/>
-    <mergeCell ref="N32:S33"/>
-    <mergeCell ref="T32:Y33"/>
-    <mergeCell ref="O25:X25"/>
-    <mergeCell ref="N26:S27"/>
-    <mergeCell ref="T26:Y27"/>
-    <mergeCell ref="O28:X28"/>
-    <mergeCell ref="N20:S21"/>
-    <mergeCell ref="T20:Y21"/>
-    <mergeCell ref="O22:X22"/>
-    <mergeCell ref="N23:S24"/>
-    <mergeCell ref="T23:Y24"/>
-    <mergeCell ref="O16:X16"/>
-    <mergeCell ref="N17:S18"/>
-    <mergeCell ref="T17:Y18"/>
-    <mergeCell ref="O19:X19"/>
-    <mergeCell ref="O13:X13"/>
-    <mergeCell ref="N14:S15"/>
-    <mergeCell ref="T14:Y15"/>
-    <mergeCell ref="N8:S9"/>
-    <mergeCell ref="T8:Y9"/>
-    <mergeCell ref="O10:X10"/>
-    <mergeCell ref="N11:S12"/>
-    <mergeCell ref="T11:Y12"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Q2:S3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="O1:S1"/>
     <mergeCell ref="N5:P6"/>
     <mergeCell ref="N2:P3"/>
     <mergeCell ref="B5:K5"/>
@@ -4144,15 +4118,35 @@
     <mergeCell ref="Q5:V6"/>
     <mergeCell ref="W2:Y3"/>
     <mergeCell ref="T2:V3"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Q2:S3"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="N8:S9"/>
+    <mergeCell ref="T8:Y9"/>
+    <mergeCell ref="O10:X10"/>
+    <mergeCell ref="N11:S12"/>
+    <mergeCell ref="T11:Y12"/>
+    <mergeCell ref="O16:X16"/>
+    <mergeCell ref="N17:S18"/>
+    <mergeCell ref="T17:Y18"/>
+    <mergeCell ref="O19:X19"/>
+    <mergeCell ref="O13:X13"/>
+    <mergeCell ref="N14:S15"/>
+    <mergeCell ref="T14:Y15"/>
+    <mergeCell ref="O25:X25"/>
+    <mergeCell ref="N26:S27"/>
+    <mergeCell ref="T26:Y27"/>
+    <mergeCell ref="O28:X28"/>
+    <mergeCell ref="N20:S21"/>
+    <mergeCell ref="T20:Y21"/>
+    <mergeCell ref="O22:X22"/>
+    <mergeCell ref="N23:S24"/>
+    <mergeCell ref="T23:Y24"/>
+    <mergeCell ref="O34:X34"/>
+    <mergeCell ref="N35:S36"/>
+    <mergeCell ref="T35:Y36"/>
+    <mergeCell ref="N29:S30"/>
+    <mergeCell ref="T29:Y30"/>
+    <mergeCell ref="O31:X31"/>
+    <mergeCell ref="N32:S33"/>
+    <mergeCell ref="T32:Y33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4161,10 +4155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4174,90 +4168,64 @@
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
         <v>162</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>160</v>
       </c>
-      <c r="D1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C12" t="s">
         <v>163</v>
       </c>
-      <c r="B7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>161</v>
-      </c>
-      <c r="C17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>